<commit_message>
upload update with vehicle
</commit_message>
<xml_diff>
--- a/worksheet.xlsx
+++ b/worksheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emad/projects/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{005B433A-D4DC-F844-93F6-F0646313B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D00BA7F9-0C54-244B-9C7F-C5D32556AE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="deepseek_csv_20251107_cbce10" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="61" uniqueCount="55">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="72" uniqueCount="50">
   <si>
     <t>riderId</t>
   </si>
@@ -163,36 +163,6 @@
     <t>Rider 10</t>
   </si>
   <si>
-    <t>E1001</t>
-  </si>
-  <si>
-    <t>E1002</t>
-  </si>
-  <si>
-    <t>E1003</t>
-  </si>
-  <si>
-    <t>E1004</t>
-  </si>
-  <si>
-    <t>E1005</t>
-  </si>
-  <si>
-    <t>E1006</t>
-  </si>
-  <si>
-    <t>E1007</t>
-  </si>
-  <si>
-    <t>E1008</t>
-  </si>
-  <si>
-    <t>E1009</t>
-  </si>
-  <si>
-    <t>E1010</t>
-  </si>
-  <si>
     <t>basicRate</t>
   </si>
   <si>
@@ -200,6 +170,21 @@
   </si>
   <si>
     <t>bonus</t>
+  </si>
+  <si>
+    <t>122336655445566</t>
+  </si>
+  <si>
+    <t>122336655445568</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>bike</t>
   </si>
 </sst>
 </file>
@@ -1048,1058 +1033,1096 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="1"/>
-    <col min="24" max="24" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="1"/>
+    <col min="25" max="25" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>26</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>189</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>82</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>107</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>3.5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>7.2</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>4</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>5</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>100</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>1057.4000000000001</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>342.15</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>265.8</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>195.5</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>625</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>45</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>15.75</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>98.2</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>185.25</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>12.5</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Z2" s="1">
         <v>35</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>250</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AB2" s="1">
         <v>340</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AC2" s="1">
         <v>75</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>120.5</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>200</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <v>342.15</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1">
         <v>500</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>31</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>215</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>65</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>150</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>3.25</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>5.35</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>4</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>5</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>1013.75</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>487.6</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>295.8</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>145</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>956</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>42.5</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>8.25</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>95.8</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>1650.8</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Y3" s="1">
         <v>5</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Z3" s="1">
         <v>45</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="1">
         <v>310</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AB3" s="1">
         <v>580</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AC3" s="1">
         <v>350</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>135.25</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AE3" s="1">
         <v>375</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AF3" s="1">
         <v>487.6</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1">
         <v>28</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>148</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>85</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>63</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>4.25</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>4.6500000000000004</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>9</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>4</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>5</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>654.20000000000005</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>215.8</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>135.5</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>125</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>132</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>35</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>38.5</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>92.5</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1">
         <v>1240.25</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Y4" s="1">
         <v>15</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Z4" s="1">
         <v>8.5</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AA4" s="1">
         <v>295</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AB4" s="1">
         <v>395</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AC4" s="1">
         <v>400</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="1">
         <v>95</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AE4" s="1">
         <v>460</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AF4" s="1">
         <v>215.8</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1">
         <v>1500</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>24</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>145</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>65</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>80</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>7.05</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>4</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>5</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>833.75</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>278.89999999999998</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>215.8</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>170.25</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>654</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>38</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>18.25</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W5" s="1">
         <v>94.2</v>
       </c>
-      <c r="W5" s="1">
+      <c r="X5" s="1">
         <v>785.6</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Y5" s="1">
         <v>7.5</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Z5" s="1">
         <v>12</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AA5" s="1">
         <v>405</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AB5" s="1">
         <v>385</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AC5" s="1">
         <v>85</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AD5" s="1">
         <v>125.75</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AE5" s="1">
         <v>42.5</v>
       </c>
-      <c r="AE5" s="1">
+      <c r="AF5" s="1">
         <v>278.89999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1">
         <v>300</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>27</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>168</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>85</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>83</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>3.55</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>6.05</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>9</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>4</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>5</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>250</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>803.9</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>312.45</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>175.8</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <v>175</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>151</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>37.5</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>35.75</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W6" s="1">
         <v>97.8</v>
       </c>
-      <c r="W6" s="1">
+      <c r="X6" s="1">
         <v>1425.8</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Y6" s="1">
         <v>20</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Z6" s="1">
         <v>25</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AA6" s="1">
         <v>335</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AB6" s="1">
         <v>605</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AC6" s="1">
         <v>290</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AD6" s="1">
         <v>98.5</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AE6" s="1">
         <v>125</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AF6" s="1">
         <v>312.45</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1">
         <v>23</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>245</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>82</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>163</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>4.6500000000000004</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>4</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>5</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>1099.25</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>421.8</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>240.25</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>150.5</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>128</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>47.5</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>42.8</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V7" s="1">
+      <c r="W7" s="1">
         <v>96.5</v>
       </c>
-      <c r="W7" s="1">
+      <c r="X7" s="1">
         <v>455.8</v>
       </c>
-      <c r="X7" s="1">
+      <c r="Y7" s="1">
         <v>10</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="Z7" s="1">
         <v>15</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AA7" s="1">
         <v>305</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AB7" s="1">
         <v>460</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AC7" s="1">
         <v>120</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AD7" s="1">
         <v>195.25</v>
       </c>
-      <c r="AD7" s="1">
+      <c r="AE7" s="1">
         <v>125</v>
       </c>
-      <c r="AE7" s="1">
+      <c r="AF7" s="1">
         <v>421.8</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1">
         <v>25</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>135</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>55</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>80</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>4.45</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>6.05</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>9</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>4</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>5</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>728.75</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>185.6</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q8" s="1">
         <v>120.8</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>160.25</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>143</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>32.5</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>5.25</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V8" s="1">
+      <c r="W8" s="1">
         <v>93.8</v>
       </c>
-      <c r="W8" s="1">
+      <c r="X8" s="1">
         <v>1725.45</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Y8" s="1">
         <v>85</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="Z8" s="1">
         <v>15</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AA8" s="1">
         <v>225</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AB8" s="1">
         <v>390</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AC8" s="1">
         <v>155</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AD8" s="1">
         <v>125.8</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AE8" s="1">
         <v>420</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AF8" s="1">
         <v>185.6</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="1">
         <v>26</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>192</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>48</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>144</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>7.15</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>4</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>5</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>1228.8</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>445.25</v>
       </c>
-      <c r="P9" s="1">
+      <c r="Q9" s="1">
         <v>225.5</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <v>115.75</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>111</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>53</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>29.5</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="1">
+      <c r="W9" s="1">
         <v>96.8</v>
       </c>
-      <c r="W9" s="1">
+      <c r="X9" s="1">
         <v>1680.25</v>
       </c>
-      <c r="X9" s="1">
+      <c r="Y9" s="1">
         <v>45</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="Z9" s="1">
         <v>18</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AA9" s="1">
         <v>245</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AB9" s="1">
         <v>600</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AC9" s="1">
         <v>320</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AD9" s="1">
         <v>42.5</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AE9" s="1">
         <v>180</v>
       </c>
-      <c r="AE9" s="1">
+      <c r="AF9" s="1">
         <v>445.25</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1">
         <v>2000</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>29</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>225</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>68</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>157</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>4.55</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>6.35</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>9</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>4</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>5</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>120</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>1306.3499999999999</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>512.79999999999995</v>
       </c>
-      <c r="P10" s="1">
+      <c r="Q10" s="1">
         <v>255.75</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <v>130</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>160</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>55</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>28.5</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V10" s="1">
+      <c r="W10" s="1">
         <v>98.5</v>
       </c>
-      <c r="W10" s="1">
+      <c r="X10" s="1">
         <v>1850.75</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Y10" s="1">
         <v>50</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="Z10" s="1">
         <v>28</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AA10" s="1">
         <v>325</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AB10" s="1">
         <v>495</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AC10" s="1">
         <v>215</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AD10" s="1">
         <v>220.8</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AE10" s="1">
         <v>85</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AF10" s="1">
         <v>512.79999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1">
         <v>26</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>142</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>50</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>92</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>3.25</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>6.25</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>9</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>4</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>5</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>300</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>737.5</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>245.6</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q11" s="1">
         <v>230.8</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <v>185.25</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>90</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>35</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>22.75</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W11" s="1">
         <v>95.5</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X11" s="1">
         <v>925.6</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Y11" s="1">
         <v>75</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Z11" s="1">
         <v>30</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AA11" s="1">
         <v>330</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AB11" s="1">
         <v>415</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AC11" s="1">
         <v>230</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AD11" s="1">
         <v>118.5</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AE11" s="1">
         <v>250</v>
       </c>
-      <c r="AE11" s="1">
+      <c r="AF11" s="1">
         <v>245.6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>